<commit_message>
train_model with prelabeled data
</commit_message>
<xml_diff>
--- a/BECT数据标注统计表.xlsx
+++ b/BECT数据标注统计表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9360"/>
+    <workbookView windowWidth="28128" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="225">
   <si>
     <t>2020.11.20</t>
   </si>
@@ -138,6 +138,9 @@
     <t>9岁3月</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>1次</t>
   </si>
   <si>
@@ -267,6 +270,9 @@
     <t>是（目测70%、80%、85%）</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>2次（2020）</t>
   </si>
   <si>
@@ -282,6 +288,9 @@
     <t>否（50、60、70）</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>3次（2021）</t>
   </si>
   <si>
@@ -321,6 +330,9 @@
     <t>否（20、25、30）</t>
   </si>
   <si>
+    <t>（1）（2）</t>
+  </si>
+  <si>
     <t>病例-15-C4-张梓骏-3段</t>
   </si>
   <si>
@@ -439,6 +451,9 @@
   </si>
   <si>
     <t>是-80、60、50</t>
+  </si>
+  <si>
+    <t>（2）（3）</t>
   </si>
   <si>
     <t>有负性肌阵挛</t>
@@ -683,31 +698,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -726,18 +727,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -748,11 +749,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -761,6 +769,14 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -779,9 +795,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -797,7 +812,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -810,33 +825,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -857,13 +865,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -875,43 +991,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -929,37 +1009,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -971,67 +1033,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1057,6 +1065,15 @@
         <color theme="4"/>
       </top>
       <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1092,15 +1109,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1111,21 +1119,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1148,141 +1141,144 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1291,15 +1287,30 @@
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1651,10 +1662,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1663,8 +1674,9 @@
     <col min="2" max="2" width="21.8888888888889" customWidth="1"/>
     <col min="3" max="3" width="12.7777777777778" customWidth="1"/>
     <col min="6" max="6" width="28.1111111111111" customWidth="1"/>
-    <col min="7" max="7" width="24.8888888888889" customWidth="1"/>
-    <col min="10" max="10" width="19.3333333333333" customWidth="1"/>
+    <col min="7" max="7" width="10.7222222222222" customWidth="1"/>
+    <col min="8" max="8" width="24.8888888888889" customWidth="1"/>
+    <col min="11" max="11" width="19.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1817,7 +1829,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1836,11 +1848,14 @@
       <c r="F12" t="s">
         <v>34</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1859,65 +1874,74 @@
       <c r="F13" t="s">
         <v>5</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
-      <c r="G14" t="s">
-        <v>45</v>
+      <c r="G14" s="1">
+        <v>3</v>
       </c>
       <c r="H14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="I14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
       </c>
       <c r="G15" s="1">
+        <v>3</v>
+      </c>
+      <c r="H15" s="2">
         <v>44319</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>33</v>
@@ -1926,82 +1950,91 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
       </c>
-      <c r="G16" t="s">
-        <v>54</v>
+      <c r="G16" s="1">
+        <v>3</v>
       </c>
       <c r="H16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
       </c>
-      <c r="G17" t="s">
-        <v>54</v>
+      <c r="G17" s="1">
+        <v>0</v>
       </c>
       <c r="H17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="I17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
       </c>
-      <c r="G18" t="s">
-        <v>54</v>
+      <c r="G18" s="1">
+        <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
-      </c>
-      <c r="J18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="K18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
@@ -2012,94 +2045,106 @@
       <c r="F19" t="s">
         <v>5</v>
       </c>
-      <c r="G19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="G19" s="1">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
       </c>
-      <c r="G20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="G20" s="1">
+        <v>3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F21" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" t="s">
-        <v>68</v>
+        <v>77</v>
+      </c>
+      <c r="G21" s="1">
+        <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>69</v>
+      </c>
+      <c r="I21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F22" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" t="s">
         <v>83</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="H22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>85</v>
+      </c>
+      <c r="I22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
         <v>3</v>
@@ -2108,116 +2153,131 @@
         <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>89</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="H24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>97</v>
+      </c>
+      <c r="I24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F25" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>103</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F26" t="s">
-        <v>104</v>
-      </c>
-      <c r="G26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>108</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F27" t="s">
-        <v>108</v>
-      </c>
-      <c r="G27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>112</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -2226,96 +2286,108 @@
         <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>113</v>
-      </c>
-      <c r="G28" t="s">
-        <v>114</v>
+        <v>117</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="H28" t="s">
-        <v>115</v>
-      </c>
-      <c r="J28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>118</v>
+      </c>
+      <c r="I28" t="s">
+        <v>119</v>
+      </c>
+      <c r="K28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D29" t="s">
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F29" t="s">
-        <v>121</v>
-      </c>
-      <c r="G29" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>125</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B30" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D30" t="s">
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
-      </c>
-      <c r="G30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>131</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C31" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D31" t="s">
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>136</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C32" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -2324,109 +2396,124 @@
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>137</v>
-      </c>
-      <c r="G32" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>141</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F33" t="s">
-        <v>140</v>
-      </c>
-      <c r="G33" t="s">
-        <v>94</v>
+        <v>144</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="H33" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>97</v>
+      </c>
+      <c r="I33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C34" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D34" t="s">
         <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F34" t="s">
-        <v>146</v>
-      </c>
-      <c r="G34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>151</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B35" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C35" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D35" t="s">
         <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F35" t="s">
-        <v>151</v>
-      </c>
-      <c r="G35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>156</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B36" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C36" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D36" t="s">
         <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="F36" t="s">
-        <v>156</v>
-      </c>
-      <c r="G36" t="s">
-        <v>40</v>
+        <v>161</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A10:H36">
+  <sortState ref="A10:I36">
     <sortCondition ref="C3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2454,262 +2541,262 @@
   <sheetData>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B11" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C13" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C14" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B16" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C16" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B17" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C17" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C18" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B19" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C20" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="B21" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C21" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B22" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C22" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B23" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B24" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C24" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C25" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B26" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C26">
         <v>2021</v>
@@ -2717,45 +2804,45 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B28" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B29" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B30" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C30" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B31" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>